<commit_message>
webshop beoordeling betere formulering
</commit_message>
<xml_diff>
--- a/2-webshop/Docent-Nakijkmodel-Webshop.xlsx
+++ b/2-webshop/Docent-Nakijkmodel-Webshop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gee/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C43826B-3AC3-B84C-A8A5-09F432F307AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C669F24-E6E0-6647-A292-BA4C30BB5E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6560" yWindow="1620" windowWidth="34560" windowHeight="19980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,12 +242,6 @@
     <t>PO Webshop HAVO</t>
   </si>
   <si>
-    <t>- Score op test met multiple-choice vragen over de basisopdrachten (hoofdstuk 2 tot en met 7, zonder uitbreidingen)
-- Je krijgt tijdens 3 lessen de gelegenheid om een test te maken. Het hoogste cijfer van de eerste 2 testen die je start telt. Als je geen test maakt (ongeacht te reden), dan is je score 0 punten.
-- Voorbereiding voor de test is het maken van de opgaven (dus geen extra leerwerk).
-- Elke leerling krijgt een eigen score voor de test (individuele beoordeling)</t>
-  </si>
-  <si>
     <t>Individuele toets in Woots. Geef 3 momenten (tijdens de les) om de toets te maken. Van de eerste twee pogingen die een leerling doet telt het hoogste cijfer. Toets niet maken is 0 punten. Doel van de test is leerlingen eruit filteren die wel de antwoorden hebben, maar niet de stof begrijpen.</t>
   </si>
   <si>
@@ -269,6 +263,9 @@
   <si>
     <t>- Geen slordigheden in opmaak
 - Logische indeling / producten vindbaar</t>
+  </si>
+  <si>
+    <t>- Score op test met multiple-choice vragen over de basisopdrachten (hoofdstuk 2 tot en met 7, zonder uitbreidingen)</t>
   </si>
 </sst>
 </file>
@@ -1931,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2033,7 +2030,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>58</v>
       </c>
@@ -2044,10 +2041,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>63</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2079,7 +2076,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="26"/>
     </row>
@@ -2129,10 +2126,10 @@
         <v>20</v>
       </c>
       <c r="D17" s="72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -2146,10 +2143,10 @@
         <v>20</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2230,6 +2227,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b60b54a5-8c6f-478f-98ee-5d9fe6b7961c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8d379a18-3696-460b-b6bd-f03ca624bc37" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB0D080B21FC2644A44B3EE466839FCA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2ee96b2c4a67ca35582eb84f7eef171">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b60b54a5-8c6f-478f-98ee-5d9fe6b7961c" xmlns:ns3="8d379a18-3696-460b-b6bd-f03ca624bc37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10eb2fa0012fee586086e9f837bf4adc" ns2:_="" ns3:_="">
     <xsd:import namespace="b60b54a5-8c6f-478f-98ee-5d9fe6b7961c"/>
@@ -2458,41 +2475,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b60b54a5-8c6f-478f-98ee-5d9fe6b7961c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8d379a18-3696-460b-b6bd-f03ca624bc37" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2482C144-BC25-4191-B417-370B72CE8CDD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{142A6AD0-5AEB-408A-90AA-477FC3B48F2C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b60b54a5-8c6f-478f-98ee-5d9fe6b7961c"/>
-    <ds:schemaRef ds:uri="8d379a18-3696-460b-b6bd-f03ca624bc37"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2515,9 +2501,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{142A6AD0-5AEB-408A-90AA-477FC3B48F2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2482C144-BC25-4191-B417-370B72CE8CDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b60b54a5-8c6f-478f-98ee-5d9fe6b7961c"/>
+    <ds:schemaRef ds:uri="8d379a18-3696-460b-b6bd-f03ca624bc37"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>